<commit_message>
adding piu cyberbulling split
</commit_message>
<xml_diff>
--- a/Data/redcap_column_names.xlsx
+++ b/Data/redcap_column_names.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\PycharmProjects\schneider-depression-lab\source\data_etl\new_process\Transferring_Data_to_PostgreSQL\column_names_mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\PycharmProjects\QuestionnaireDashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t>questionnaire_name</t>
   </si>
@@ -230,12 +230,6 @@
     <t>ecrrc_timestamp,erc_rc_1,erc_rc_2,erc_rc_3,erc_rc_4,erc_rc_5,erc_rc_6,erc_rc_7,erc_rc_8,erc_rc_9,erc_rc_10,erc_rc_11,erc_rc_12</t>
   </si>
   <si>
-    <t>piu_cyberbulling</t>
-  </si>
-  <si>
-    <t>piu_cyberbulling_timestamp,piu_1,piu_2,piu_3,piu_4,piu_5,piu_6,cyberbulling_1,cyberbulling_2,cyberbulling_3,cyberbulling_4,cyberbulling_5,cyberbulling_6,cyberbulling_7,cyberbulling_8,cyberbulling_9,cyberbulling_10,cyberbulling_11,bullied_1,bullied_2,bullied_3,bullied_4</t>
-  </si>
-  <si>
     <t>erq_ca</t>
   </si>
   <si>
@@ -522,6 +516,18 @@
   </si>
   <si>
     <t>record_id,redcap_event_name,redcap_survey_identifier</t>
+  </si>
+  <si>
+    <t>piu</t>
+  </si>
+  <si>
+    <t>cyberbulling</t>
+  </si>
+  <si>
+    <t>cyberbulling_1,cyberbulling_2,cyberbulling_3,cyberbulling_4,cyberbulling_5,cyberbulling_6,cyberbulling_7,cyberbulling_8,cyberbulling_9,cyberbulling_10,cyberbulling_11,bullied_1,bullied_2,bullied_3,bullied_4</t>
+  </si>
+  <si>
+    <t>piu_cyberbulling_timestamp,piu_1,piu_2,piu_3,piu_4,piu_5,piu_6</t>
   </si>
 </sst>
 </file>
@@ -591,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -607,6 +613,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -889,15 +898,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E165"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A32" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.08203125" customWidth="1"/>
+    <col min="2" max="2" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23" x14ac:dyDescent="0.3">
@@ -1252,7 +1262,7 @@
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
     </row>
-    <row r="33" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>64</v>
       </c>
@@ -1274,122 +1284,122 @@
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
-    <row r="35" spans="1:5" ht="57.5" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>69</v>
+    <row r="35" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
     </row>
-    <row r="36" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>71</v>
+    <row r="36" spans="1:5" ht="46" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
     </row>
-    <row r="37" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
     </row>
-    <row r="38" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
     </row>
-    <row r="39" spans="1:5" ht="126.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
     </row>
-    <row r="40" spans="1:5" ht="138" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="126.5" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
     </row>
-    <row r="41" spans="1:5" ht="57.5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="138" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
-    <row r="42" spans="1:5" ht="115" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="57.5" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
     </row>
-    <row r="43" spans="1:5" ht="80.5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="115" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
     </row>
-    <row r="44" spans="1:5" ht="115" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="80.5" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="115" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
@@ -1397,10 +1407,10 @@
     </row>
     <row r="46" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -1408,120 +1418,120 @@
     </row>
     <row r="47" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
-    <row r="48" spans="1:5" ht="57.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="57.5" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
     </row>
-    <row r="50" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
     </row>
-    <row r="51" spans="1:5" ht="138" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
     </row>
-    <row r="52" spans="1:5" ht="253" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="138" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
     </row>
-    <row r="53" spans="1:5" ht="287.5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="253" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
     </row>
-    <row r="54" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="287.5" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
     </row>
-    <row r="55" spans="1:5" ht="276" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
     </row>
-    <row r="56" spans="1:5" ht="218.5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="276" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
     </row>
-    <row r="57" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="218.5" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -1529,32 +1539,32 @@
     </row>
     <row r="58" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
       <c r="E58" s="5"/>
     </row>
-    <row r="59" spans="1:5" ht="57.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
     </row>
-    <row r="60" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="57.5" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -1562,65 +1572,65 @@
     </row>
     <row r="61" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
     </row>
-    <row r="62" spans="1:5" ht="103.5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
     </row>
-    <row r="63" spans="1:5" ht="126.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="103.5" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="126.5" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
     </row>
-    <row r="65" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -1628,10 +1638,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -1639,10 +1649,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
@@ -1650,10 +1660,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
@@ -1661,65 +1671,65 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
     </row>
-    <row r="71" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
     </row>
-    <row r="72" spans="1:5" ht="46" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
     </row>
-    <row r="73" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="46" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
     </row>
-    <row r="74" spans="1:5" ht="57.5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
       <c r="E74" s="5"/>
     </row>
-    <row r="75" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="57.5" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
@@ -1727,10 +1737,10 @@
     </row>
     <row r="76" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
@@ -1738,10 +1748,10 @@
     </row>
     <row r="77" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
@@ -1749,10 +1759,10 @@
     </row>
     <row r="78" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
@@ -1760,62 +1770,69 @@
     </row>
     <row r="79" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
       <c r="E79" s="5"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="5"/>
     </row>
-    <row r="81" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
       <c r="E81" s="5"/>
     </row>
-    <row r="82" spans="1:5" ht="34.5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="23" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B83" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
+    <row r="83" spans="1:5" ht="23" x14ac:dyDescent="0.3">
+      <c r="A83" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
+      <c r="A84" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
@@ -2138,8 +2155,12 @@
       <c r="B164" s="1"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" s="2"/>
-      <c r="B165" s="2"/>
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A166" s="2"/>
+      <c r="B166" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>